<commit_message>
docs: Added missing file in spread sheet
Added in spread sheet
spmu298d.pdf
</commit_message>
<xml_diff>
--- a/ManualsDatasheets/ManualsDataSheetsSpreadsheet.xlsx
+++ b/ManualsDatasheets/ManualsDataSheetsSpreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20339"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5338BF51-5309-4BA9-A433-CD1D07AED275}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961FDFBA-BB40-4904-9E37-C16923C7BD8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Document</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>tm4c123gh6pm.pdf</t>
+  </si>
+  <si>
+    <t>User's Guide</t>
+  </si>
+  <si>
+    <t>TivaWare Peripheral Driver Library</t>
+  </si>
+  <si>
+    <t>spmu298d.pdf</t>
   </si>
 </sst>
 </file>
@@ -414,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -513,6 +522,20 @@
         <v>20</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
docs: Actual Tiva TM4C123GH6PM Microcontroller
Adding new file:
tm4c123gh6pm2014.pdf

and actualizing spreadsheet.
</commit_message>
<xml_diff>
--- a/ManualsDatasheets/ManualsDataSheetsSpreadsheet.xlsx
+++ b/ManualsDatasheets/ManualsDataSheetsSpreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20339"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961FDFBA-BB40-4904-9E37-C16923C7BD8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C87496-061B-414A-91B9-6AA83D217DC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Document</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>spmu298d.pdf</t>
+  </si>
+  <si>
+    <t>tm4c123gh6pm2014.pdf</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,6 +539,20 @@
         <v>23</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
docs: Adding new document 'CortexM4 Technical Reference Manual'
Adding new file:
'CortexM4_TRM_r0p1.pdf'

Also updating the spreadsheet.
</commit_message>
<xml_diff>
--- a/ManualsDatasheets/ManualsDataSheetsSpreadsheet.xlsx
+++ b/ManualsDatasheets/ManualsDataSheetsSpreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20339"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C87496-061B-414A-91B9-6AA83D217DC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2AB9A8-2B0B-4E95-A8C1-D4AA490C15E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Document</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>tm4c123gh6pm2014.pdf</t>
+  </si>
+  <si>
+    <t>Corte-M4 Revision r0p1</t>
+  </si>
+  <si>
+    <t>Cortex-M4 Revision r0p1</t>
+  </si>
+  <si>
+    <t>CortexM4_TRM_r0p1</t>
   </si>
 </sst>
 </file>
@@ -426,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -553,6 +562,20 @@
         <v>24</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
docs: Adding Documentation Generic Users Guide Cortex-M4 Devices       Completing Data Sheet
Addding new file:
'DUI0553.pdf'

Also updating the spreadsheet.
</commit_message>
<xml_diff>
--- a/ManualsDatasheets/ManualsDataSheetsSpreadsheet.xlsx
+++ b/ManualsDatasheets/ManualsDataSheetsSpreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20339"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2AB9A8-2B0B-4E95-A8C1-D4AA490C15E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38DA931-EB0A-4FA1-B00E-42FB3064593B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="17625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>Document</t>
   </si>
@@ -104,6 +104,15 @@
   </si>
   <si>
     <t>CortexM4_TRM_r0p1</t>
+  </si>
+  <si>
+    <t>Generic User Guiede</t>
+  </si>
+  <si>
+    <t>Cortex-M4 Devices</t>
+  </si>
+  <si>
+    <t>DUI0553.pdf</t>
   </si>
 </sst>
 </file>
@@ -435,22 +444,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.08984375" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
     <col min="2" max="2" width="27" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29.54296875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="49.08984375" customWidth="1"/>
-    <col min="5" max="5" width="21.6328125" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="49.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -478,7 +487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -492,7 +501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -506,7 +515,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -520,7 +529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -534,7 +543,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -548,7 +557,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -562,7 +571,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -574,6 +583,17 @@
       </c>
       <c r="D9" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>